<commit_message>
Mean Values and Box Plot Section
</commit_message>
<xml_diff>
--- a/Experiment Output/Jan/Format/ANCHOR_XAI_Metrics_Experiments Formatted cf v1-0 290124.xlsx
+++ b/Experiment Output/Jan/Format/ANCHOR_XAI_Metrics_Experiments Formatted cf v1-0 290124.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\T_UD\Dissertation\PreWork_Repo\Dissertation_PreWork\Experiment Output\Jan\Format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47A7921-7B04-400F-A6C9-44AC295BE5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3059B2BA-7518-4B2C-A818-B87CB0C2699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71880" yWindow="-4290" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-4815" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ANCHOR" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -45,7 +45,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -187,16 +187,16 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -516,7 +516,7 @@
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>